<commit_message>
Longest substring without repeating character
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B135401-1248-3649-998A-3BB60C3C51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
-    <sheet r:id="rId2" sheetId="2" name="DW"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DW" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$G$14</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
   <si>
     <t/>
   </si>
@@ -294,13 +300,21 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Coin Change</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/coin-change/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic programming bottm up approach start by calculating dp to complete 1 ruppe then 2 ruppes then so onn </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -318,7 +332,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9c5700"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -330,7 +344,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
       <family val="2"/>
     </font>
@@ -351,16 +365,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffeb9c"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFc6efce"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -377,58 +391,71 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -439,10 +466,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="335B74"/>
@@ -480,71 +507,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -572,7 +599,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -595,11 +622,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -608,13 +635,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -624,7 +651,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -633,7 +660,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -642,7 +669,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -650,10 +677,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -718,7 +745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -726,18 +753,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="6" width="43.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="71.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="108.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="43.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="108.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -760,7 +786,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>39</v>
       </c>
@@ -781,7 +807,7 @@
       </c>
       <c r="G2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>44</v>
       </c>
@@ -802,7 +828,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
@@ -823,7 +849,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>50</v>
       </c>
@@ -844,7 +870,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -865,7 +891,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
@@ -886,7 +912,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>60</v>
       </c>
@@ -907,7 +933,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
@@ -918,7 +944,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>64</v>
       </c>
@@ -939,7 +965,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>67</v>
       </c>
@@ -960,7 +986,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>70</v>
       </c>
@@ -981,7 +1007,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>73</v>
       </c>
@@ -1002,7 +1028,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>75</v>
       </c>
@@ -1023,7 +1049,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>78</v>
       </c>
@@ -1044,7 +1070,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>81</v>
       </c>
@@ -1065,7 +1091,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>84</v>
       </c>
@@ -1086,7 +1112,7 @@
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>87</v>
       </c>
@@ -1107,7 +1133,7 @@
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1116,7 +1142,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1125,7 +1151,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1134,7 +1160,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1145,7 +1171,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1154,7 +1180,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1163,7 +1189,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1172,7 +1198,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1189,24 +1215,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="6" width="32.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="53.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="110.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="32.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110.5" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1223,14 +1251,14 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1264,7 +1292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -1281,7 +1309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -1298,7 +1326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -1315,7 +1343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -1332,7 +1360,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -1349,7 +1377,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1364,6 +1392,23 @@
       </c>
       <c r="E10" s="4" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validate binary search tree
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26F36A7-9696-7A49-A415-C8FAB5C4E32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323BF6CE-520B-3F4C-B90F-5ECA645C9B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
   <si>
     <t/>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>Start calculating the subsequence from last number and come down to last and return max of listt</t>
+  </si>
+  <si>
+    <t>Validate Binary search Tree</t>
+  </si>
+  <si>
+    <t>Take inf on both ends and then compare and move</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -495,6 +501,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1272,10 +1281,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1515,6 +1524,23 @@
         <v>103</v>
       </c>
     </row>
+    <row r="15" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove Spaces from String
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323BF6CE-520B-3F4C-B90F-5ECA645C9B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5797349-6420-A743-A8BE-62A68B16F2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="109">
   <si>
     <t/>
   </si>
@@ -343,6 +343,15 @@
   </si>
   <si>
     <t>Take inf on both ends and then compare and move</t>
+  </si>
+  <si>
+    <t>Remove Spaces from string</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/remove-spaces-from-a-given-string/</t>
+  </si>
+  <si>
+    <t>Traverse and only add no space characters in a list and then join the list to a empty string</t>
   </si>
 </sst>
 </file>
@@ -1281,10 +1290,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="A15:XFD15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1541,6 +1550,23 @@
         <v>105</v>
       </c>
     </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
n th largest element in an array
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5797349-6420-A743-A8BE-62A68B16F2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A7868-AE13-DE4D-9FD7-B0C3C3DAE3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="112">
   <si>
     <t/>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>Traverse and only add no space characters in a list and then join the list to a empty string</t>
+  </si>
+  <si>
+    <t>Kth largest element in an array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-largest-element-in-an-array/</t>
+  </si>
+  <si>
+    <t>quick select algo using partition</t>
   </si>
 </sst>
 </file>
@@ -431,7 +440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -472,13 +481,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -511,6 +529,12 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1290,10 +1314,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1550,21 +1574,38 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:5" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="16" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Power of a number'
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADB6A9B-D210-7D41-928B-B90D72C846F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFEF0B6-1075-7243-A82A-D75836038112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
   <si>
     <t/>
   </si>
@@ -361,6 +361,24 @@
   </si>
   <si>
     <t>quick select algo using partition</t>
+  </si>
+  <si>
+    <t>Middle of inked List</t>
+  </si>
+  <si>
+    <t>Slow and fast pointer</t>
+  </si>
+  <si>
+    <t>PowerOf AnotherNumber</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/check-if-a-number-is-power-of-another-number</t>
+  </si>
+  <si>
+    <t>Check by multiplying the number again and again</t>
   </si>
 </sst>
 </file>
@@ -496,7 +514,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -535,6 +553,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1306,6 +1327,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1314,10 +1336,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1608,8 +1630,43 @@
         <v>111</v>
       </c>
     </row>
+    <row r="18" spans="1:5" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merge two linked list
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,27 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFEF0B6-1075-7243-A82A-D75836038112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1687BAA3-57CE-274D-AF7C-CF7268FD557A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DW" sheetId="2" r:id="rId2"/>
+    <sheet name="DW" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DW!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$G$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$18</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
   <si>
     <t>Problem type</t>
   </si>
@@ -379,6 +376,24 @@
   </si>
   <si>
     <t>Check by multiplying the number again and again</t>
+  </si>
+  <si>
+    <t>MirrorTree</t>
+  </si>
+  <si>
+    <t>Start with providing a recursive function with two values root,root then compare in cross faishon</t>
+  </si>
+  <si>
+    <t>Merge Two Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-sorted-lists/</t>
+  </si>
+  <si>
+    <t>Problem Statement</t>
+  </si>
+  <si>
+    <t>Create a dummy linked list first then keep checking which num is smaller and keep adding to that . In rest if any list is left append it</t>
   </si>
 </sst>
 </file>
@@ -514,7 +529,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -540,12 +555,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -867,7 +880,9 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -881,177 +896,177 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1062,190 +1077,190 @@
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="F18" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -1282,7 +1297,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1319,354 +1334,384 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G18" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C7A26D-AA6D-524D-A908-2C7B2F6EB298}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="110.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.5" customWidth="1"/>
+    <col min="4" max="4" width="60.1640625" customWidth="1"/>
+    <col min="5" max="5" width="109.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="E11" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E13" s="12" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="E14" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="D16" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="16" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="B17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="17" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="B18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="18" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="18" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>117</v>
       </c>
+      <c r="B20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:E1" xr:uid="{81C7A26D-AA6D-524D-A908-2C7B2F6EB298}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reverse Linked List easy
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD33521-F76C-5E48-A400-8D1B9E7CAA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEAB84C-94D4-6E47-A297-E47F102650C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="26880" windowHeight="15260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="155">
   <si>
     <t>Problem type</t>
   </si>
@@ -481,6 +481,15 @@
   </si>
   <si>
     <t>if else and ans when of the the one is equal to root or there is a split</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Palindrom Substring</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/distinct-palindromic-substrings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just add a list to check for repeating </t>
   </si>
 </sst>
 </file>
@@ -1439,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C7A26D-AA6D-524D-A908-2C7B2F6EB298}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1819,7 +1828,7 @@
     </row>
     <row r="23" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>26</v>
@@ -1968,6 +1977,23 @@
       </c>
       <c r="E31" s="15" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverse Linked List of k node easy version
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEAB84C-94D4-6E47-A297-E47F102650C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D969F0-916C-484B-B634-9AA62D2E4D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="158">
   <si>
     <t>Problem type</t>
   </si>
@@ -490,6 +490,15 @@
   </si>
   <si>
     <t xml:space="preserve">Just add a list to check for repeating </t>
+  </si>
+  <si>
+    <t>Reverse a Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/</t>
+  </si>
+  <si>
+    <t>Use a prev=None pointer and keep changing the next pos</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C7A26D-AA6D-524D-A908-2C7B2F6EB298}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1996,6 +2005,23 @@
         <v>154</v>
       </c>
     </row>
+    <row r="33" spans="1:5" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{81C7A26D-AA6D-524D-A908-2C7B2F6EB298}"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Check for circular linked list
</commit_message>
<xml_diff>
--- a/Problem Solving.xlsx
+++ b/Problem Solving.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i532970/problemSolving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D969F0-916C-484B-B634-9AA62D2E4D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2922B943-7B2E-414E-8204-5E9D597B2C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="161">
   <si>
     <t>Problem type</t>
   </si>
@@ -499,6 +499,15 @@
   </si>
   <si>
     <t>Use a prev=None pointer and keep changing the next pos</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/reverse-a-linked-list-in-groups-of-given-size</t>
+  </si>
+  <si>
+    <t>use reccursion with normal reversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse a Linked List of K version easy one </t>
   </si>
 </sst>
 </file>
@@ -1457,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C7A26D-AA6D-524D-A908-2C7B2F6EB298}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2022,6 +2031,23 @@
         <v>157</v>
       </c>
     </row>
+    <row r="34" spans="1:5" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{81C7A26D-AA6D-524D-A908-2C7B2F6EB298}"/>
   <hyperlinks>

</xml_diff>